<commit_message>
Added results from pairwise comparisons for alpha & beta div
</commit_message>
<xml_diff>
--- a/saved_stats.xlsx
+++ b/saved_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\Cecum_Microbes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3649813F-6C78-42E7-9546-14E6B4D334BB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49A8C54-AB46-45B0-BC31-07809B65ECAC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{76FDAE5B-2FE0-4081-8A14-9A02BDD15C6B}"/>
   </bookViews>
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F641FC-ECF0-4FEE-B1F4-8B1BE68EF1BC}">
   <dimension ref="A1:P105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="P65" sqref="P65"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71:B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>